<commit_message>
Changed RegExp for more universale user input
</commit_message>
<xml_diff>
--- a/Datasetv2.xlsx
+++ b/Datasetv2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Justin S\Experiments\Growth Rate\Cell Cycle Length Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Justin_S\Experiments\Growth Rate\Cell Cycle Length Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="0" windowWidth="23550" windowHeight="11265"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="185">
   <si>
     <t>Path to Dataset</t>
   </si>
@@ -214,9 +214,6 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171024_JS_p27_68HrRESULTS</t>
   </si>
   <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx</t>
-  </si>
-  <si>
     <t>20171024_JS_p27</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_16HrRESULTS</t>
   </si>
   <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx</t>
-  </si>
-  <si>
     <t>20171030_JS_p27</t>
   </si>
   <si>
@@ -490,9 +484,6 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171121_JS_p27_cycE_66HrRESULTS</t>
   </si>
   <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx</t>
-  </si>
-  <si>
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171121_JS_p27_cycE_0HrRESULTS</t>
   </si>
   <si>
@@ -506,6 +497,84 @@
   </si>
   <si>
     <t>p27, cycE</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_0HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_6HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_21HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_30HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_45HrRESULTS</t>
+  </si>
+  <si>
+    <t>20171204_JS_cycE</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_54HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_70HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_70Hr_SERESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_0HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_8HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_19HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_0HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_8HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_19HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20180108_cycE1_P27.xlsx</t>
+  </si>
+  <si>
+    <t>20180108_JS_cycE</t>
+  </si>
+  <si>
+    <t>20180108_JS_p27</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_28HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_28HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_45HrRESULTS</t>
+  </si>
+  <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_45HrRESULTS</t>
   </si>
 </sst>
 </file>
@@ -837,8 +906,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K111" totalsRowShown="0">
-  <autoFilter ref="A1:K111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K129" totalsRowShown="0">
+  <autoFilter ref="A1:K129"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Path to Dataset" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" name="Plate_Map" dataCellStyle="Hyperlink"/>
@@ -1119,17 +1188,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105:D111"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
@@ -1154,7 +1223,7 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
@@ -1169,7 +1238,7 @@
         <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1177,22 +1246,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" t="s">
-        <v>118</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -1201,10 +1270,10 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K2" s="2">
         <v>42892</v>
@@ -1212,22 +1281,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
         <v>116</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>118</v>
       </c>
       <c r="G3" s="5">
         <v>7</v>
@@ -1236,10 +1305,10 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K3" s="2">
         <v>42892</v>
@@ -1247,22 +1316,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
         <v>116</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>118</v>
       </c>
       <c r="G4" s="5">
         <v>20</v>
@@ -1271,10 +1340,10 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K4" s="2">
         <v>42892</v>
@@ -1282,22 +1351,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
         <v>116</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>118</v>
       </c>
       <c r="G5" s="5">
         <v>32</v>
@@ -1306,10 +1375,10 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K5" s="2">
         <v>42892</v>
@@ -1317,22 +1386,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
         <v>116</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>118</v>
       </c>
       <c r="G6" s="5">
         <v>46</v>
@@ -1341,10 +1410,10 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K6" s="2">
         <v>42892</v>
@@ -1352,22 +1421,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
         <v>116</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>118</v>
       </c>
       <c r="G7" s="5">
         <v>57</v>
@@ -1376,10 +1445,10 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K7" s="2">
         <v>42892</v>
@@ -1387,23 +1456,23 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>118</v>
-      </c>
       <c r="G8" s="6">
         <v>70</v>
       </c>
@@ -1411,10 +1480,10 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K8" s="2">
         <v>42892</v>
@@ -1422,22 +1491,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
         <v>116</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" t="s">
-        <v>118</v>
       </c>
       <c r="G9" s="5">
         <v>77</v>
@@ -1446,10 +1515,10 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K9" s="2">
         <v>42892</v>
@@ -1457,22 +1526,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
         <v>116</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" t="s">
-        <v>118</v>
       </c>
       <c r="G10" s="5">
         <v>57</v>
@@ -1481,10 +1550,10 @@
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K10" s="2">
         <v>42892</v>
@@ -1492,22 +1561,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
         <v>116</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>118</v>
       </c>
       <c r="G11" s="5">
         <v>77</v>
@@ -1516,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K11" s="2">
         <v>42892</v>
@@ -1527,22 +1596,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G12" s="7">
         <v>0</v>
@@ -1551,10 +1620,10 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K12" s="2">
         <v>42913</v>
@@ -1562,22 +1631,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G13" s="7">
         <v>15</v>
@@ -1586,10 +1655,10 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2">
         <v>42913</v>
@@ -1597,22 +1666,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G14" s="7">
         <v>25</v>
@@ -1621,10 +1690,10 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2">
         <v>42913</v>
@@ -1632,22 +1701,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G15" s="7">
         <v>46</v>
@@ -1656,10 +1725,10 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K15" s="2">
         <v>42913</v>
@@ -1667,22 +1736,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G16" s="7">
         <v>53</v>
@@ -1691,10 +1760,10 @@
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K16" s="2">
         <v>42913</v>
@@ -1702,22 +1771,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G17" s="7">
         <v>71</v>
@@ -1726,10 +1795,10 @@
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K17" s="2">
         <v>42913</v>
@@ -1737,22 +1806,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G18" s="5">
         <v>52</v>
@@ -1761,10 +1830,10 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K18" s="2">
         <v>42913</v>
@@ -1772,22 +1841,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G19" s="5">
         <v>71</v>
@@ -1796,10 +1865,10 @@
         <v>4</v>
       </c>
       <c r="I19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K19" s="2">
         <v>42913</v>
@@ -1807,22 +1876,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G20" s="7">
         <v>0</v>
@@ -1831,10 +1900,10 @@
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K20" s="2">
         <v>42913</v>
@@ -1842,22 +1911,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G21" s="7">
         <v>15</v>
@@ -1866,10 +1935,10 @@
         <v>4</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K21" s="2">
         <v>42913</v>
@@ -1877,22 +1946,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G22" s="7">
         <v>25</v>
@@ -1901,10 +1970,10 @@
         <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K22" s="2">
         <v>42913</v>
@@ -1912,22 +1981,22 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G23" s="7">
         <v>46</v>
@@ -1936,10 +2005,10 @@
         <v>4</v>
       </c>
       <c r="I23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K23" s="2">
         <v>42913</v>
@@ -1947,22 +2016,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G24" s="7">
         <v>53</v>
@@ -1971,10 +2040,10 @@
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K24" s="2">
         <v>42913</v>
@@ -1982,22 +2051,22 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G25" s="7">
         <v>71</v>
@@ -2006,10 +2075,10 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K25" s="2">
         <v>42913</v>
@@ -2017,22 +2086,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G26" s="5">
         <v>53</v>
@@ -2041,10 +2110,10 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K26" s="2">
         <v>42913</v>
@@ -2052,22 +2121,22 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G27" s="5">
         <v>71</v>
@@ -2076,10 +2145,10 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K27" s="2">
         <v>42913</v>
@@ -2099,7 +2168,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
@@ -2111,10 +2180,10 @@
         <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K28" s="2">
         <v>43004</v>
@@ -2134,7 +2203,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -2146,10 +2215,10 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K29" s="2">
         <v>43004</v>
@@ -2169,7 +2238,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
@@ -2181,10 +2250,10 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K30" s="2">
         <v>43004</v>
@@ -2204,7 +2273,7 @@
         <v>22</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -2216,10 +2285,10 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K31" s="2">
         <v>43004</v>
@@ -2239,7 +2308,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -2251,10 +2320,10 @@
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K32" s="2">
         <v>43004</v>
@@ -2274,7 +2343,7 @@
         <v>22</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -2286,10 +2355,10 @@
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K33" s="2">
         <v>43004</v>
@@ -2297,7 +2366,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
@@ -2309,7 +2378,7 @@
         <v>22</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
@@ -2321,10 +2390,10 @@
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K34" s="2">
         <v>43004</v>
@@ -2344,7 +2413,7 @@
         <v>23</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2356,10 +2425,10 @@
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K35" s="2">
         <v>43004</v>
@@ -2379,7 +2448,7 @@
         <v>23</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -2391,10 +2460,10 @@
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K36" s="2">
         <v>43004</v>
@@ -2414,7 +2483,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -2426,10 +2495,10 @@
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K37" s="2">
         <v>43004</v>
@@ -2449,7 +2518,7 @@
         <v>23</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -2461,10 +2530,10 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K38" s="2">
         <v>43004</v>
@@ -2484,7 +2553,7 @@
         <v>23</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -2496,10 +2565,10 @@
         <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K39" s="2">
         <v>43004</v>
@@ -2519,7 +2588,7 @@
         <v>23</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -2531,10 +2600,10 @@
         <v>4</v>
       </c>
       <c r="I40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K40" s="2">
         <v>43004</v>
@@ -2542,7 +2611,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>37</v>
@@ -2554,7 +2623,7 @@
         <v>23</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -2566,10 +2635,10 @@
         <v>4</v>
       </c>
       <c r="I41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K41" s="2">
         <v>43004</v>
@@ -2589,7 +2658,7 @@
         <v>22</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F42" t="s">
         <v>33</v>
@@ -2601,10 +2670,10 @@
         <v>4</v>
       </c>
       <c r="I42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K42" s="2">
         <v>43011</v>
@@ -2624,7 +2693,7 @@
         <v>22</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" t="s">
         <v>33</v>
@@ -2636,10 +2705,10 @@
         <v>4</v>
       </c>
       <c r="I43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K43" s="2">
         <v>43011</v>
@@ -2659,7 +2728,7 @@
         <v>22</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" t="s">
         <v>33</v>
@@ -2671,10 +2740,10 @@
         <v>4</v>
       </c>
       <c r="I44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K44" s="2">
         <v>43011</v>
@@ -2682,7 +2751,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>38</v>
@@ -2694,7 +2763,7 @@
         <v>22</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45" t="s">
         <v>33</v>
@@ -2706,10 +2775,10 @@
         <v>4</v>
       </c>
       <c r="I45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K45" s="2">
         <v>43011</v>
@@ -2717,7 +2786,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>38</v>
@@ -2729,7 +2798,7 @@
         <v>22</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F46" t="s">
         <v>33</v>
@@ -2741,10 +2810,10 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K46" s="2">
         <v>43011</v>
@@ -2764,7 +2833,7 @@
         <v>23</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" t="s">
         <v>34</v>
@@ -2776,10 +2845,10 @@
         <v>4</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K47" s="2">
         <v>43011</v>
@@ -2799,7 +2868,7 @@
         <v>23</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -2811,10 +2880,10 @@
         <v>4</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K48" s="2">
         <v>43011</v>
@@ -2834,7 +2903,7 @@
         <v>23</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -2846,10 +2915,10 @@
         <v>4</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K49" s="2">
         <v>43011</v>
@@ -2857,7 +2926,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>38</v>
@@ -2869,7 +2938,7 @@
         <v>23</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F50" t="s">
         <v>34</v>
@@ -2881,10 +2950,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K50" s="2">
         <v>43011</v>
@@ -2892,7 +2961,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>38</v>
@@ -2904,7 +2973,7 @@
         <v>23</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51" t="s">
         <v>34</v>
@@ -2916,10 +2985,10 @@
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K51" s="2">
         <v>43011</v>
@@ -2939,7 +3008,7 @@
         <v>36</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" t="s">
         <v>35</v>
@@ -2954,7 +3023,7 @@
         <v>40</v>
       </c>
       <c r="J52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K52" s="2">
         <v>43011</v>
@@ -2974,7 +3043,7 @@
         <v>36</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" t="s">
         <v>35</v>
@@ -2989,7 +3058,7 @@
         <v>40</v>
       </c>
       <c r="J53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K53" s="2">
         <v>43011</v>
@@ -3009,7 +3078,7 @@
         <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F54" t="s">
         <v>35</v>
@@ -3024,7 +3093,7 @@
         <v>40</v>
       </c>
       <c r="J54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K54" s="2">
         <v>43011</v>
@@ -3032,7 +3101,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>38</v>
@@ -3044,7 +3113,7 @@
         <v>36</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F55" t="s">
         <v>35</v>
@@ -3059,7 +3128,7 @@
         <v>40</v>
       </c>
       <c r="J55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K55" s="2">
         <v>43011</v>
@@ -3067,7 +3136,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>38</v>
@@ -3079,7 +3148,7 @@
         <v>36</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" t="s">
         <v>35</v>
@@ -3094,7 +3163,7 @@
         <v>40</v>
       </c>
       <c r="J56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K56" s="2">
         <v>43011</v>
@@ -3105,7 +3174,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>21</v>
@@ -3114,10 +3183,10 @@
         <v>22</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G57" s="5">
         <v>0</v>
@@ -3126,10 +3195,10 @@
         <v>4</v>
       </c>
       <c r="I57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K57" s="2">
         <v>43032</v>
@@ -3140,7 +3209,7 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>21</v>
@@ -3149,10 +3218,10 @@
         <v>22</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G58" s="5">
         <v>18</v>
@@ -3161,10 +3230,10 @@
         <v>4</v>
       </c>
       <c r="I58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K58" s="2">
         <v>43032</v>
@@ -3175,7 +3244,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -3184,10 +3253,10 @@
         <v>22</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G59" s="5">
         <v>24</v>
@@ -3196,10 +3265,10 @@
         <v>4</v>
       </c>
       <c r="I59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J59" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K59" s="2">
         <v>43032</v>
@@ -3210,7 +3279,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>21</v>
@@ -3219,10 +3288,10 @@
         <v>22</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G60" s="5">
         <v>42</v>
@@ -3231,10 +3300,10 @@
         <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K60" s="2">
         <v>43032</v>
@@ -3245,7 +3314,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>21</v>
@@ -3254,10 +3323,10 @@
         <v>22</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G61" s="5">
         <v>48</v>
@@ -3266,10 +3335,10 @@
         <v>4</v>
       </c>
       <c r="I61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J61" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K61" s="2">
         <v>43032</v>
@@ -3280,7 +3349,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>21</v>
@@ -3289,10 +3358,10 @@
         <v>22</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G62" s="5">
         <v>63</v>
@@ -3301,10 +3370,10 @@
         <v>4</v>
       </c>
       <c r="I62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K62" s="2">
         <v>43032</v>
@@ -3315,7 +3384,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>21</v>
@@ -3324,10 +3393,10 @@
         <v>22</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G63" s="5">
         <v>69</v>
@@ -3336,10 +3405,10 @@
         <v>4</v>
       </c>
       <c r="I63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K63" s="2">
         <v>43032</v>
@@ -3347,10 +3416,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>21</v>
@@ -3359,10 +3428,10 @@
         <v>22</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G64" s="5">
         <v>69</v>
@@ -3371,10 +3440,10 @@
         <v>4</v>
       </c>
       <c r="I64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J64" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K64" s="2">
         <v>43032</v>
@@ -3385,19 +3454,19 @@
         <v>50</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G65" s="5">
         <v>0</v>
@@ -3406,10 +3475,10 @@
         <v>4</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J65" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K65" s="2">
         <v>43032</v>
@@ -3420,19 +3489,19 @@
         <v>51</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G66" s="5">
         <v>18</v>
@@ -3441,10 +3510,10 @@
         <v>4</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K66" s="2">
         <v>43032</v>
@@ -3455,19 +3524,19 @@
         <v>52</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G67" s="5">
         <v>24</v>
@@ -3476,10 +3545,10 @@
         <v>4</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K67" s="2">
         <v>43032</v>
@@ -3490,19 +3559,19 @@
         <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G68" s="5">
         <v>42</v>
@@ -3511,10 +3580,10 @@
         <v>4</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K68" s="2">
         <v>43032</v>
@@ -3525,19 +3594,19 @@
         <v>54</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G69" s="5">
         <v>48</v>
@@ -3546,10 +3615,10 @@
         <v>4</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J69" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K69" s="2">
         <v>43032</v>
@@ -3560,19 +3629,19 @@
         <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G70" s="5">
         <v>63</v>
@@ -3581,10 +3650,10 @@
         <v>4</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J70" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K70" s="2">
         <v>43032</v>
@@ -3595,19 +3664,19 @@
         <v>56</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G71" s="5">
         <v>69</v>
@@ -3616,10 +3685,10 @@
         <v>4</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J71" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K71" s="2">
         <v>43032</v>
@@ -3627,22 +3696,22 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G72" s="5">
         <v>69</v>
@@ -3651,10 +3720,10 @@
         <v>4</v>
       </c>
       <c r="I72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J72" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K72" s="2">
         <v>43032</v>
@@ -3665,19 +3734,19 @@
         <v>57</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" t="s">
         <v>64</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F73" t="s">
-        <v>65</v>
       </c>
       <c r="G73" s="5">
         <v>0</v>
@@ -3689,7 +3758,7 @@
         <v>40</v>
       </c>
       <c r="J73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K73" s="2">
         <v>43032</v>
@@ -3700,19 +3769,19 @@
         <v>58</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F74" t="s">
         <v>64</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F74" t="s">
-        <v>65</v>
       </c>
       <c r="G74" s="5">
         <v>18</v>
@@ -3724,7 +3793,7 @@
         <v>40</v>
       </c>
       <c r="J74" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K74" s="2">
         <v>43032</v>
@@ -3735,19 +3804,19 @@
         <v>59</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F75" t="s">
         <v>64</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F75" t="s">
-        <v>65</v>
       </c>
       <c r="G75" s="5">
         <v>24</v>
@@ -3759,7 +3828,7 @@
         <v>40</v>
       </c>
       <c r="J75" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K75" s="2">
         <v>43032</v>
@@ -3770,19 +3839,19 @@
         <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" t="s">
         <v>64</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F76" t="s">
-        <v>65</v>
       </c>
       <c r="G76" s="5">
         <v>42</v>
@@ -3794,7 +3863,7 @@
         <v>40</v>
       </c>
       <c r="J76" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K76" s="2">
         <v>43032</v>
@@ -3805,19 +3874,19 @@
         <v>61</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F77" t="s">
         <v>64</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F77" t="s">
-        <v>65</v>
       </c>
       <c r="G77" s="5">
         <v>48</v>
@@ -3829,7 +3898,7 @@
         <v>40</v>
       </c>
       <c r="J77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K77" s="2">
         <v>43032</v>
@@ -3840,19 +3909,19 @@
         <v>62</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F78" t="s">
         <v>64</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F78" t="s">
-        <v>65</v>
       </c>
       <c r="G78" s="5">
         <v>63</v>
@@ -3864,7 +3933,7 @@
         <v>40</v>
       </c>
       <c r="J78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K78" s="2">
         <v>43032</v>
@@ -3875,19 +3944,19 @@
         <v>63</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79" t="s">
         <v>64</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F79" t="s">
-        <v>65</v>
       </c>
       <c r="G79" s="5">
         <v>69</v>
@@ -3899,7 +3968,7 @@
         <v>40</v>
       </c>
       <c r="J79" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K79" s="2">
         <v>43032</v>
@@ -3907,22 +3976,22 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F80" t="s">
         <v>64</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F80" t="s">
-        <v>65</v>
       </c>
       <c r="G80" s="5">
         <v>69</v>
@@ -3934,7 +4003,7 @@
         <v>40</v>
       </c>
       <c r="J80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K80" s="2">
         <v>43032</v>
@@ -3942,22 +4011,22 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G81" s="5">
         <v>0</v>
@@ -3969,7 +4038,7 @@
         <v>40</v>
       </c>
       <c r="J81" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K81" s="2">
         <v>43038</v>
@@ -3977,22 +4046,22 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G82" s="5">
         <v>16</v>
@@ -4004,7 +4073,7 @@
         <v>40</v>
       </c>
       <c r="J82" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K82" s="2">
         <v>43038</v>
@@ -4012,22 +4081,22 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F83" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G83" s="5">
         <v>21</v>
@@ -4039,7 +4108,7 @@
         <v>40</v>
       </c>
       <c r="J83" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K83" s="2">
         <v>43038</v>
@@ -4047,22 +4116,22 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F84" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G84" s="5">
         <v>26</v>
@@ -4074,7 +4143,7 @@
         <v>40</v>
       </c>
       <c r="J84" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K84" s="2">
         <v>43038</v>
@@ -4082,22 +4151,22 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F85" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G85" s="5">
         <v>42</v>
@@ -4109,7 +4178,7 @@
         <v>40</v>
       </c>
       <c r="J85" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K85" s="2">
         <v>43038</v>
@@ -4117,22 +4186,22 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F86" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G86" s="5">
         <v>47</v>
@@ -4144,7 +4213,7 @@
         <v>40</v>
       </c>
       <c r="J86" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K86" s="2">
         <v>43038</v>
@@ -4152,22 +4221,22 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F87" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G87" s="5">
         <v>66</v>
@@ -4179,7 +4248,7 @@
         <v>40</v>
       </c>
       <c r="J87" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K87" s="2">
         <v>43038</v>
@@ -4187,22 +4256,22 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F88" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G88" s="5">
         <v>66</v>
@@ -4214,7 +4283,7 @@
         <v>40</v>
       </c>
       <c r="J88" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K88" s="2">
         <v>43038</v>
@@ -4222,22 +4291,22 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F89" t="s">
         <v>80</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F89" t="s">
-        <v>82</v>
       </c>
       <c r="G89" s="5">
         <v>0</v>
@@ -4246,10 +4315,10 @@
         <v>4</v>
       </c>
       <c r="I89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J89" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K89" s="2">
         <v>43038</v>
@@ -4257,22 +4326,22 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F90" t="s">
         <v>80</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F90" t="s">
-        <v>82</v>
       </c>
       <c r="G90" s="5">
         <v>16</v>
@@ -4281,10 +4350,10 @@
         <v>4</v>
       </c>
       <c r="I90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J90" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K90" s="2">
         <v>43038</v>
@@ -4292,23 +4361,23 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F91" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F91" t="s">
-        <v>82</v>
-      </c>
       <c r="G91" s="5">
         <v>21</v>
       </c>
@@ -4316,10 +4385,10 @@
         <v>4</v>
       </c>
       <c r="I91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J91" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K91" s="2">
         <v>43038</v>
@@ -4327,22 +4396,22 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" t="s">
         <v>80</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F92" t="s">
-        <v>82</v>
       </c>
       <c r="G92" s="5">
         <v>26</v>
@@ -4351,10 +4420,10 @@
         <v>4</v>
       </c>
       <c r="I92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J92" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K92" s="2">
         <v>43038</v>
@@ -4362,22 +4431,22 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F93" t="s">
         <v>80</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F93" t="s">
-        <v>82</v>
       </c>
       <c r="G93" s="5">
         <v>42</v>
@@ -4386,10 +4455,10 @@
         <v>4</v>
       </c>
       <c r="I93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J93" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K93" s="2">
         <v>43038</v>
@@ -4397,22 +4466,22 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F94" t="s">
         <v>80</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F94" t="s">
-        <v>82</v>
       </c>
       <c r="G94" s="5">
         <v>47</v>
@@ -4421,10 +4490,10 @@
         <v>4</v>
       </c>
       <c r="I94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J94" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K94" s="2">
         <v>43038</v>
@@ -4432,22 +4501,22 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F95" t="s">
         <v>80</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F95" t="s">
-        <v>82</v>
       </c>
       <c r="G95" s="5">
         <v>66</v>
@@ -4456,10 +4525,10 @@
         <v>4</v>
       </c>
       <c r="I95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K95" s="2">
         <v>43038</v>
@@ -4467,22 +4536,22 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F96" t="s">
         <v>80</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F96" t="s">
-        <v>82</v>
       </c>
       <c r="G96" s="5">
         <v>66</v>
@@ -4491,10 +4560,10 @@
         <v>4</v>
       </c>
       <c r="I96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J96" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K96" s="2">
         <v>43038</v>
@@ -4502,10 +4571,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>21</v>
@@ -4514,10 +4583,10 @@
         <v>22</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F97" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G97" s="5">
         <v>0</v>
@@ -4526,10 +4595,10 @@
         <v>4</v>
       </c>
       <c r="I97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J97" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K97" s="2">
         <v>43038</v>
@@ -4537,10 +4606,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>21</v>
@@ -4549,10 +4618,10 @@
         <v>22</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F98" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G98" s="5">
         <v>16</v>
@@ -4561,10 +4630,10 @@
         <v>4</v>
       </c>
       <c r="I98" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J98" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K98" s="2">
         <v>43038</v>
@@ -4572,10 +4641,10 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>21</v>
@@ -4584,22 +4653,22 @@
         <v>22</v>
       </c>
       <c r="E99" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F99" t="s">
+        <v>81</v>
+      </c>
+      <c r="G99" s="5">
+        <v>21</v>
+      </c>
+      <c r="H99" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99" t="s">
         <v>71</v>
       </c>
-      <c r="F99" t="s">
-        <v>83</v>
-      </c>
-      <c r="G99" s="5">
-        <v>21</v>
-      </c>
-      <c r="H99" t="s">
-        <v>4</v>
-      </c>
-      <c r="I99" t="s">
-        <v>72</v>
-      </c>
       <c r="J99" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K99" s="2">
         <v>43038</v>
@@ -4607,10 +4676,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>21</v>
@@ -4619,10 +4688,10 @@
         <v>22</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F100" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G100" s="5">
         <v>26</v>
@@ -4631,10 +4700,10 @@
         <v>4</v>
       </c>
       <c r="I100" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J100" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K100" s="2">
         <v>43038</v>
@@ -4642,10 +4711,10 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>21</v>
@@ -4654,10 +4723,10 @@
         <v>22</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G101" s="5">
         <v>42</v>
@@ -4666,10 +4735,10 @@
         <v>4</v>
       </c>
       <c r="I101" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J101" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K101" s="2">
         <v>43038</v>
@@ -4677,10 +4746,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>21</v>
@@ -4689,10 +4758,10 @@
         <v>22</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F102" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G102" s="5">
         <v>47</v>
@@ -4701,10 +4770,10 @@
         <v>4</v>
       </c>
       <c r="I102" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J102" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K102" s="2">
         <v>43038</v>
@@ -4712,10 +4781,10 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>21</v>
@@ -4724,10 +4793,10 @@
         <v>22</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F103" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G103" s="5">
         <v>66</v>
@@ -4736,10 +4805,10 @@
         <v>4</v>
       </c>
       <c r="I103" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K103" s="2">
         <v>43038</v>
@@ -4747,10 +4816,10 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>21</v>
@@ -4759,10 +4828,10 @@
         <v>22</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F104" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G104" s="5">
         <v>66</v>
@@ -4771,10 +4840,10 @@
         <v>4</v>
       </c>
       <c r="I104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J104" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K104" s="2">
         <v>43038</v>
@@ -4782,22 +4851,22 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F105" t="s">
         <v>157</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F105" t="s">
-        <v>160</v>
       </c>
       <c r="G105" s="5">
         <v>0</v>
@@ -4806,10 +4875,10 @@
         <v>4</v>
       </c>
       <c r="I105" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K105" s="2">
         <v>43060</v>
@@ -4817,22 +4886,22 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F106" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G106" s="5">
         <v>8</v>
@@ -4841,10 +4910,10 @@
         <v>4</v>
       </c>
       <c r="I106" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J106" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K106" s="2">
         <v>43060</v>
@@ -4852,22 +4921,22 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F107" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G107" s="5">
         <v>21</v>
@@ -4876,10 +4945,10 @@
         <v>4</v>
       </c>
       <c r="I107" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J107" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K107" s="2">
         <v>43060</v>
@@ -4887,22 +4956,22 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F108" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G108" s="5">
         <v>30</v>
@@ -4911,10 +4980,10 @@
         <v>4</v>
       </c>
       <c r="I108" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J108" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K108" s="2">
         <v>43060</v>
@@ -4922,22 +4991,22 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F109" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G109" s="5">
         <v>45</v>
@@ -4946,10 +5015,10 @@
         <v>4</v>
       </c>
       <c r="I109" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J109" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K109" s="2">
         <v>43060</v>
@@ -4957,22 +5026,22 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F110" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G110" s="5">
         <v>54</v>
@@ -4981,10 +5050,10 @@
         <v>4</v>
       </c>
       <c r="I110" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J110" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K110" s="2">
         <v>43060</v>
@@ -4992,22 +5061,22 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F111" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G111" s="5">
         <v>66</v>
@@ -5016,13 +5085,643 @@
         <v>4</v>
       </c>
       <c r="I111" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J111" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K111" s="2">
         <v>43060</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F112" t="s">
+        <v>164</v>
+      </c>
+      <c r="G112" s="5">
+        <v>0</v>
+      </c>
+      <c r="H112" t="s">
+        <v>4</v>
+      </c>
+      <c r="I112" t="s">
+        <v>72</v>
+      </c>
+      <c r="J112" t="s">
+        <v>101</v>
+      </c>
+      <c r="K112" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F113" t="s">
+        <v>164</v>
+      </c>
+      <c r="G113" s="5">
+        <v>6</v>
+      </c>
+      <c r="H113" t="s">
+        <v>4</v>
+      </c>
+      <c r="I113" t="s">
+        <v>72</v>
+      </c>
+      <c r="J113" t="s">
+        <v>101</v>
+      </c>
+      <c r="K113" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F114" t="s">
+        <v>164</v>
+      </c>
+      <c r="G114" s="5">
+        <v>21</v>
+      </c>
+      <c r="H114" t="s">
+        <v>4</v>
+      </c>
+      <c r="I114" t="s">
+        <v>72</v>
+      </c>
+      <c r="J114" t="s">
+        <v>101</v>
+      </c>
+      <c r="K114" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F115" t="s">
+        <v>164</v>
+      </c>
+      <c r="G115" s="5">
+        <v>30</v>
+      </c>
+      <c r="H115" t="s">
+        <v>4</v>
+      </c>
+      <c r="I115" t="s">
+        <v>72</v>
+      </c>
+      <c r="J115" t="s">
+        <v>101</v>
+      </c>
+      <c r="K115" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F116" t="s">
+        <v>164</v>
+      </c>
+      <c r="G116" s="5">
+        <v>45</v>
+      </c>
+      <c r="H116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I116" t="s">
+        <v>72</v>
+      </c>
+      <c r="J116" t="s">
+        <v>101</v>
+      </c>
+      <c r="K116" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F117" t="s">
+        <v>164</v>
+      </c>
+      <c r="G117" s="5">
+        <v>54</v>
+      </c>
+      <c r="H117" t="s">
+        <v>4</v>
+      </c>
+      <c r="I117" t="s">
+        <v>72</v>
+      </c>
+      <c r="J117" t="s">
+        <v>101</v>
+      </c>
+      <c r="K117" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F118" t="s">
+        <v>164</v>
+      </c>
+      <c r="G118" s="5">
+        <v>70</v>
+      </c>
+      <c r="H118" t="s">
+        <v>4</v>
+      </c>
+      <c r="I118" t="s">
+        <v>72</v>
+      </c>
+      <c r="J118" t="s">
+        <v>101</v>
+      </c>
+      <c r="K118" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F119" t="s">
+        <v>164</v>
+      </c>
+      <c r="G119" s="5">
+        <v>70</v>
+      </c>
+      <c r="H119" t="s">
+        <v>4</v>
+      </c>
+      <c r="I119" t="s">
+        <v>72</v>
+      </c>
+      <c r="J119" t="s">
+        <v>113</v>
+      </c>
+      <c r="K119" s="2">
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F120" t="s">
+        <v>179</v>
+      </c>
+      <c r="G120" s="5">
+        <v>0</v>
+      </c>
+      <c r="H120" t="s">
+        <v>4</v>
+      </c>
+      <c r="I120" t="s">
+        <v>72</v>
+      </c>
+      <c r="J120" t="s">
+        <v>101</v>
+      </c>
+      <c r="K120" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F121" t="s">
+        <v>179</v>
+      </c>
+      <c r="G121" s="5">
+        <v>8</v>
+      </c>
+      <c r="H121" t="s">
+        <v>4</v>
+      </c>
+      <c r="I121" t="s">
+        <v>72</v>
+      </c>
+      <c r="J121" t="s">
+        <v>101</v>
+      </c>
+      <c r="K121" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F122" t="s">
+        <v>179</v>
+      </c>
+      <c r="G122" s="5">
+        <v>19</v>
+      </c>
+      <c r="H122" t="s">
+        <v>4</v>
+      </c>
+      <c r="I122" t="s">
+        <v>72</v>
+      </c>
+      <c r="J122" t="s">
+        <v>101</v>
+      </c>
+      <c r="K122" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F123" t="s">
+        <v>179</v>
+      </c>
+      <c r="G123" s="5">
+        <v>28</v>
+      </c>
+      <c r="H123" t="s">
+        <v>4</v>
+      </c>
+      <c r="I123" t="s">
+        <v>72</v>
+      </c>
+      <c r="J123" t="s">
+        <v>101</v>
+      </c>
+      <c r="K123" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F124" t="s">
+        <v>179</v>
+      </c>
+      <c r="G124" s="5">
+        <v>45</v>
+      </c>
+      <c r="H124" t="s">
+        <v>4</v>
+      </c>
+      <c r="I124" t="s">
+        <v>72</v>
+      </c>
+      <c r="J124" t="s">
+        <v>101</v>
+      </c>
+      <c r="K124" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F125" t="s">
+        <v>180</v>
+      </c>
+      <c r="G125" s="5">
+        <v>0</v>
+      </c>
+      <c r="H125" t="s">
+        <v>4</v>
+      </c>
+      <c r="I125" t="s">
+        <v>40</v>
+      </c>
+      <c r="J125" t="s">
+        <v>101</v>
+      </c>
+      <c r="K125" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F126" t="s">
+        <v>180</v>
+      </c>
+      <c r="G126" s="5">
+        <v>8</v>
+      </c>
+      <c r="H126" t="s">
+        <v>4</v>
+      </c>
+      <c r="I126" t="s">
+        <v>40</v>
+      </c>
+      <c r="J126" t="s">
+        <v>101</v>
+      </c>
+      <c r="K126" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F127" t="s">
+        <v>180</v>
+      </c>
+      <c r="G127" s="5">
+        <v>19</v>
+      </c>
+      <c r="H127" t="s">
+        <v>4</v>
+      </c>
+      <c r="I127" t="s">
+        <v>40</v>
+      </c>
+      <c r="J127" t="s">
+        <v>101</v>
+      </c>
+      <c r="K127" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F128" t="s">
+        <v>180</v>
+      </c>
+      <c r="G128" s="5">
+        <v>28</v>
+      </c>
+      <c r="H128" t="s">
+        <v>4</v>
+      </c>
+      <c r="I128" t="s">
+        <v>40</v>
+      </c>
+      <c r="J128" t="s">
+        <v>101</v>
+      </c>
+      <c r="K128" s="2">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F129" t="s">
+        <v>180</v>
+      </c>
+      <c r="G129" s="5">
+        <v>45</v>
+      </c>
+      <c r="H129" t="s">
+        <v>4</v>
+      </c>
+      <c r="I129" t="s">
+        <v>40</v>
+      </c>
+      <c r="J129" t="s">
+        <v>101</v>
+      </c>
+      <c r="K129" s="2">
+        <v>43108</v>
       </c>
     </row>
   </sheetData>
@@ -5039,15 +5738,15 @@
     <hyperlink ref="A73" r:id="rId10"/>
     <hyperlink ref="A78" r:id="rId11"/>
     <hyperlink ref="A79" r:id="rId12"/>
-    <hyperlink ref="B57" r:id="rId13"/>
+    <hyperlink ref="B57" r:id="rId13" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
     <hyperlink ref="A89" r:id="rId14"/>
-    <hyperlink ref="B81" r:id="rId15"/>
+    <hyperlink ref="B81" r:id="rId15" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
     <hyperlink ref="A81" r:id="rId16"/>
     <hyperlink ref="A97" r:id="rId17"/>
     <hyperlink ref="A28" r:id="rId18"/>
     <hyperlink ref="B2" r:id="rId19"/>
     <hyperlink ref="B34" r:id="rId20"/>
-    <hyperlink ref="B104" r:id="rId21"/>
+    <hyperlink ref="B104" r:id="rId21" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
     <hyperlink ref="A2" r:id="rId22"/>
     <hyperlink ref="A3" r:id="rId23"/>
     <hyperlink ref="A12" r:id="rId24" display="\\carbon.research.sickkids.ca\OPRETTA\Operetta Processed OutPutFiles\Dataset_20170627_HD_CycD_6hrRESULTS"/>
@@ -5083,12 +5782,12 @@
     <hyperlink ref="A10" r:id="rId54"/>
     <hyperlink ref="A19" r:id="rId55"/>
     <hyperlink ref="A20" r:id="rId56"/>
-    <hyperlink ref="B67" r:id="rId57"/>
-    <hyperlink ref="B65" r:id="rId58"/>
-    <hyperlink ref="B95" r:id="rId59"/>
+    <hyperlink ref="B67" r:id="rId57" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B65" r:id="rId58" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B95" r:id="rId59" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
     <hyperlink ref="B29" r:id="rId60"/>
     <hyperlink ref="A106" r:id="rId61"/>
-    <hyperlink ref="B105" r:id="rId62"/>
+    <hyperlink ref="B105" r:id="rId62" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx"/>
     <hyperlink ref="B106:B111" r:id="rId63" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx"/>
     <hyperlink ref="A104" r:id="rId64"/>
     <hyperlink ref="A105" r:id="rId65"/>
@@ -5097,11 +5796,27 @@
     <hyperlink ref="A109" r:id="rId68"/>
     <hyperlink ref="A110" r:id="rId69"/>
     <hyperlink ref="A111" r:id="rId70"/>
+    <hyperlink ref="B112" r:id="rId71" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
+    <hyperlink ref="A112" r:id="rId72"/>
+    <hyperlink ref="B117" r:id="rId73" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
+    <hyperlink ref="B118" r:id="rId74" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
+    <hyperlink ref="B119" r:id="rId75" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
+    <hyperlink ref="A119" r:id="rId76"/>
+    <hyperlink ref="A122" r:id="rId77"/>
+    <hyperlink ref="A125" r:id="rId78"/>
+    <hyperlink ref="B120" r:id="rId79"/>
+    <hyperlink ref="B121:B127" r:id="rId80" display="\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20180108_cycE1_P27.xlsx"/>
+    <hyperlink ref="A120" r:id="rId81"/>
+    <hyperlink ref="A126" r:id="rId82"/>
+    <hyperlink ref="B123" r:id="rId83"/>
+    <hyperlink ref="B128" r:id="rId84"/>
+    <hyperlink ref="B124" r:id="rId85"/>
+    <hyperlink ref="B129" r:id="rId86"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId87"/>
   <tableParts count="1">
-    <tablePart r:id="rId72"/>
+    <tablePart r:id="rId88"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Revert previous commit 33a2e35ccdc91295e2d996b0789e534b9e446d51: Revert "Changed RegExp for more universale user input"
This reverts commit 33a2e35ccdc91295e2d996b0789e534b9e446d51.
</commit_message>
<xml_diff>
--- a/Datasetv2.xlsx
+++ b/Datasetv2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Justin_S\Experiments\Growth Rate\Cell Cycle Length Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Justin S\Experiments\Growth Rate\Cell Cycle Length Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="18600" yWindow="0" windowWidth="23550" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="162">
   <si>
     <t>Path to Dataset</t>
   </si>
@@ -214,6 +214,9 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171024_JS_p27_68HrRESULTS</t>
   </si>
   <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx</t>
+  </si>
+  <si>
     <t>20171024_JS_p27</t>
   </si>
   <si>
@@ -259,6 +262,9 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171030_JS_cycD_16HrRESULTS</t>
   </si>
   <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx</t>
+  </si>
+  <si>
     <t>20171030_JS_p27</t>
   </si>
   <si>
@@ -484,6 +490,9 @@
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171121_JS_p27_cycE_66HrRESULTS</t>
   </si>
   <si>
+    <t>\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx</t>
+  </si>
+  <si>
     <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171121_JS_p27_cycE_0HrRESULTS</t>
   </si>
   <si>
@@ -497,84 +506,6 @@
   </si>
   <si>
     <t>p27, cycE</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_0HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_6HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_21HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_30HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_45HrRESULTS</t>
-  </si>
-  <si>
-    <t>20171204_JS_cycE</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_54HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_70HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20171204_JS_cycE_70Hr_SERESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_0HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_8HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_19HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_0HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_8HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_19HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20180108_cycE1_P27.xlsx</t>
-  </si>
-  <si>
-    <t>20180108_JS_cycE</t>
-  </si>
-  <si>
-    <t>20180108_JS_p27</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_28HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_28HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_cycE_45HrRESULTS</t>
-  </si>
-  <si>
-    <t>\\carbon.research.sickkids.ca\rkafri\OPRETTA\Operetta Processed OutPutFiles\Dataset_20180108_JS_p27_45HrRESULTS</t>
   </si>
 </sst>
 </file>
@@ -906,8 +837,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K129" totalsRowShown="0">
-  <autoFilter ref="A1:K129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K111" totalsRowShown="0">
+  <autoFilter ref="A1:K111"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Path to Dataset" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" name="Plate_Map" dataCellStyle="Hyperlink"/>
@@ -1188,17 +1119,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="69" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
@@ -1223,7 +1154,7 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
@@ -1238,7 +1169,7 @@
         <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1246,22 +1177,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -1270,10 +1201,10 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2">
         <v>42892</v>
@@ -1281,22 +1212,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G3" s="5">
         <v>7</v>
@@ -1305,10 +1236,10 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2">
         <v>42892</v>
@@ -1316,22 +1247,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G4" s="5">
         <v>20</v>
@@ -1340,10 +1271,10 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K4" s="2">
         <v>42892</v>
@@ -1351,22 +1282,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G5" s="5">
         <v>32</v>
@@ -1375,10 +1306,10 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K5" s="2">
         <v>42892</v>
@@ -1386,22 +1317,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G6" s="5">
         <v>46</v>
@@ -1410,10 +1341,10 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K6" s="2">
         <v>42892</v>
@@ -1421,22 +1352,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G7" s="5">
         <v>57</v>
@@ -1445,10 +1376,10 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K7" s="2">
         <v>42892</v>
@@ -1456,22 +1387,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G8" s="6">
         <v>70</v>
@@ -1480,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K8" s="2">
         <v>42892</v>
@@ -1491,22 +1422,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G9" s="5">
         <v>77</v>
@@ -1515,10 +1446,10 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K9" s="2">
         <v>42892</v>
@@ -1526,22 +1457,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G10" s="5">
         <v>57</v>
@@ -1550,10 +1481,10 @@
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K10" s="2">
         <v>42892</v>
@@ -1561,22 +1492,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
         <v>118</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>116</v>
       </c>
       <c r="G11" s="5">
         <v>77</v>
@@ -1585,10 +1516,10 @@
         <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J11" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K11" s="2">
         <v>42892</v>
@@ -1596,22 +1527,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G12" s="7">
         <v>0</v>
@@ -1620,10 +1551,10 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2">
         <v>42913</v>
@@ -1631,22 +1562,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G13" s="7">
         <v>15</v>
@@ -1655,10 +1586,10 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K13" s="2">
         <v>42913</v>
@@ -1666,22 +1597,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G14" s="7">
         <v>25</v>
@@ -1690,10 +1621,10 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K14" s="2">
         <v>42913</v>
@@ -1701,22 +1632,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G15" s="7">
         <v>46</v>
@@ -1725,10 +1656,10 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K15" s="2">
         <v>42913</v>
@@ -1736,22 +1667,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G16" s="7">
         <v>53</v>
@@ -1760,10 +1691,10 @@
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K16" s="2">
         <v>42913</v>
@@ -1771,22 +1702,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G17" s="7">
         <v>71</v>
@@ -1795,10 +1726,10 @@
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K17" s="2">
         <v>42913</v>
@@ -1806,22 +1737,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G18" s="5">
         <v>52</v>
@@ -1830,10 +1761,10 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K18" s="2">
         <v>42913</v>
@@ -1841,23 +1772,23 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" t="s">
-        <v>121</v>
-      </c>
       <c r="G19" s="5">
         <v>71</v>
       </c>
@@ -1865,10 +1796,10 @@
         <v>4</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K19" s="2">
         <v>42913</v>
@@ -1876,22 +1807,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G20" s="7">
         <v>0</v>
@@ -1900,10 +1831,10 @@
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K20" s="2">
         <v>42913</v>
@@ -1911,22 +1842,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G21" s="7">
         <v>15</v>
@@ -1935,10 +1866,10 @@
         <v>4</v>
       </c>
       <c r="I21" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K21" s="2">
         <v>42913</v>
@@ -1946,22 +1877,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" t="s">
         <v>145</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>143</v>
       </c>
       <c r="G22" s="7">
         <v>25</v>
@@ -1970,10 +1901,10 @@
         <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K22" s="2">
         <v>42913</v>
@@ -1981,22 +1912,22 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G23" s="7">
         <v>46</v>
@@ -2005,10 +1936,10 @@
         <v>4</v>
       </c>
       <c r="I23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K23" s="2">
         <v>42913</v>
@@ -2016,22 +1947,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G24" s="7">
         <v>53</v>
@@ -2040,10 +1971,10 @@
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K24" s="2">
         <v>42913</v>
@@ -2051,22 +1982,22 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G25" s="7">
         <v>71</v>
@@ -2075,10 +2006,10 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K25" s="2">
         <v>42913</v>
@@ -2086,22 +2017,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G26" s="5">
         <v>53</v>
@@ -2110,10 +2041,10 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K26" s="2">
         <v>42913</v>
@@ -2121,22 +2052,22 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G27" s="5">
         <v>71</v>
@@ -2145,10 +2076,10 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K27" s="2">
         <v>42913</v>
@@ -2168,7 +2099,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
@@ -2180,10 +2111,10 @@
         <v>4</v>
       </c>
       <c r="I28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J28" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K28" s="2">
         <v>43004</v>
@@ -2203,7 +2134,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -2215,10 +2146,10 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J29" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K29" s="2">
         <v>43004</v>
@@ -2238,7 +2169,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
@@ -2250,10 +2181,10 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K30" s="2">
         <v>43004</v>
@@ -2273,7 +2204,7 @@
         <v>22</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -2285,10 +2216,10 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K31" s="2">
         <v>43004</v>
@@ -2308,7 +2239,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -2320,10 +2251,10 @@
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K32" s="2">
         <v>43004</v>
@@ -2343,7 +2274,7 @@
         <v>22</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -2355,10 +2286,10 @@
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K33" s="2">
         <v>43004</v>
@@ -2366,7 +2297,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
@@ -2378,7 +2309,7 @@
         <v>22</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
@@ -2390,10 +2321,10 @@
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J34" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K34" s="2">
         <v>43004</v>
@@ -2413,7 +2344,7 @@
         <v>23</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2425,10 +2356,10 @@
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J35" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K35" s="2">
         <v>43004</v>
@@ -2448,7 +2379,7 @@
         <v>23</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -2460,10 +2391,10 @@
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J36" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K36" s="2">
         <v>43004</v>
@@ -2483,7 +2414,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -2495,10 +2426,10 @@
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J37" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K37" s="2">
         <v>43004</v>
@@ -2518,7 +2449,7 @@
         <v>23</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -2530,10 +2461,10 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J38" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K38" s="2">
         <v>43004</v>
@@ -2553,7 +2484,7 @@
         <v>23</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -2565,10 +2496,10 @@
         <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J39" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K39" s="2">
         <v>43004</v>
@@ -2588,7 +2519,7 @@
         <v>23</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -2600,10 +2531,10 @@
         <v>4</v>
       </c>
       <c r="I40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J40" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K40" s="2">
         <v>43004</v>
@@ -2611,7 +2542,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>37</v>
@@ -2623,7 +2554,7 @@
         <v>23</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -2635,10 +2566,10 @@
         <v>4</v>
       </c>
       <c r="I41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J41" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K41" s="2">
         <v>43004</v>
@@ -2658,7 +2589,7 @@
         <v>22</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F42" t="s">
         <v>33</v>
@@ -2670,10 +2601,10 @@
         <v>4</v>
       </c>
       <c r="I42" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J42" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K42" s="2">
         <v>43011</v>
@@ -2693,7 +2624,7 @@
         <v>22</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
         <v>33</v>
@@ -2705,10 +2636,10 @@
         <v>4</v>
       </c>
       <c r="I43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J43" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K43" s="2">
         <v>43011</v>
@@ -2728,7 +2659,7 @@
         <v>22</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F44" t="s">
         <v>33</v>
@@ -2740,10 +2671,10 @@
         <v>4</v>
       </c>
       <c r="I44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K44" s="2">
         <v>43011</v>
@@ -2751,7 +2682,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>38</v>
@@ -2763,7 +2694,7 @@
         <v>22</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F45" t="s">
         <v>33</v>
@@ -2775,10 +2706,10 @@
         <v>4</v>
       </c>
       <c r="I45" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J45" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K45" s="2">
         <v>43011</v>
@@ -2786,7 +2717,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>38</v>
@@ -2798,7 +2729,7 @@
         <v>22</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F46" t="s">
         <v>33</v>
@@ -2810,10 +2741,10 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K46" s="2">
         <v>43011</v>
@@ -2833,7 +2764,7 @@
         <v>23</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
         <v>34</v>
@@ -2845,10 +2776,10 @@
         <v>4</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J47" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K47" s="2">
         <v>43011</v>
@@ -2868,7 +2799,7 @@
         <v>23</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -2880,10 +2811,10 @@
         <v>4</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J48" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K48" s="2">
         <v>43011</v>
@@ -2903,7 +2834,7 @@
         <v>23</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -2915,10 +2846,10 @@
         <v>4</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J49" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K49" s="2">
         <v>43011</v>
@@ -2926,7 +2857,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>38</v>
@@ -2938,7 +2869,7 @@
         <v>23</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
         <v>34</v>
@@ -2950,10 +2881,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J50" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K50" s="2">
         <v>43011</v>
@@ -2961,7 +2892,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>38</v>
@@ -2973,7 +2904,7 @@
         <v>23</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
         <v>34</v>
@@ -2985,10 +2916,10 @@
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J51" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K51" s="2">
         <v>43011</v>
@@ -3008,7 +2939,7 @@
         <v>36</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F52" t="s">
         <v>35</v>
@@ -3023,7 +2954,7 @@
         <v>40</v>
       </c>
       <c r="J52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K52" s="2">
         <v>43011</v>
@@ -3043,7 +2974,7 @@
         <v>36</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F53" t="s">
         <v>35</v>
@@ -3058,7 +2989,7 @@
         <v>40</v>
       </c>
       <c r="J53" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K53" s="2">
         <v>43011</v>
@@ -3078,7 +3009,7 @@
         <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F54" t="s">
         <v>35</v>
@@ -3093,7 +3024,7 @@
         <v>40</v>
       </c>
       <c r="J54" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K54" s="2">
         <v>43011</v>
@@ -3101,7 +3032,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>38</v>
@@ -3113,7 +3044,7 @@
         <v>36</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F55" t="s">
         <v>35</v>
@@ -3128,7 +3059,7 @@
         <v>40</v>
       </c>
       <c r="J55" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K55" s="2">
         <v>43011</v>
@@ -3136,7 +3067,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>38</v>
@@ -3148,7 +3079,7 @@
         <v>36</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F56" t="s">
         <v>35</v>
@@ -3163,7 +3094,7 @@
         <v>40</v>
       </c>
       <c r="J56" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K56" s="2">
         <v>43011</v>
@@ -3174,7 +3105,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>21</v>
@@ -3183,10 +3114,10 @@
         <v>22</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G57" s="5">
         <v>0</v>
@@ -3195,10 +3126,10 @@
         <v>4</v>
       </c>
       <c r="I57" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J57" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K57" s="2">
         <v>43032</v>
@@ -3209,7 +3140,7 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>21</v>
@@ -3218,10 +3149,10 @@
         <v>22</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F58" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G58" s="5">
         <v>18</v>
@@ -3230,10 +3161,10 @@
         <v>4</v>
       </c>
       <c r="I58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J58" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K58" s="2">
         <v>43032</v>
@@ -3244,7 +3175,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -3253,10 +3184,10 @@
         <v>22</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G59" s="5">
         <v>24</v>
@@ -3265,10 +3196,10 @@
         <v>4</v>
       </c>
       <c r="I59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J59" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K59" s="2">
         <v>43032</v>
@@ -3279,7 +3210,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>21</v>
@@ -3288,10 +3219,10 @@
         <v>22</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F60" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G60" s="5">
         <v>42</v>
@@ -3300,10 +3231,10 @@
         <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K60" s="2">
         <v>43032</v>
@@ -3314,7 +3245,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>21</v>
@@ -3323,10 +3254,10 @@
         <v>22</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F61" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G61" s="5">
         <v>48</v>
@@ -3335,10 +3266,10 @@
         <v>4</v>
       </c>
       <c r="I61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J61" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K61" s="2">
         <v>43032</v>
@@ -3349,7 +3280,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>21</v>
@@ -3358,10 +3289,10 @@
         <v>22</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G62" s="5">
         <v>63</v>
@@ -3370,10 +3301,10 @@
         <v>4</v>
       </c>
       <c r="I62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J62" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K62" s="2">
         <v>43032</v>
@@ -3384,7 +3315,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>21</v>
@@ -3393,10 +3324,10 @@
         <v>22</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G63" s="5">
         <v>69</v>
@@ -3405,10 +3336,10 @@
         <v>4</v>
       </c>
       <c r="I63" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J63" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K63" s="2">
         <v>43032</v>
@@ -3416,10 +3347,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>21</v>
@@ -3428,10 +3359,10 @@
         <v>22</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G64" s="5">
         <v>69</v>
@@ -3440,10 +3371,10 @@
         <v>4</v>
       </c>
       <c r="I64" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J64" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K64" s="2">
         <v>43032</v>
@@ -3454,19 +3385,19 @@
         <v>50</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" t="s">
         <v>67</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F65" t="s">
-        <v>66</v>
       </c>
       <c r="G65" s="5">
         <v>0</v>
@@ -3475,10 +3406,10 @@
         <v>4</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J65" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K65" s="2">
         <v>43032</v>
@@ -3489,19 +3420,19 @@
         <v>51</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" t="s">
         <v>67</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F66" t="s">
-        <v>66</v>
       </c>
       <c r="G66" s="5">
         <v>18</v>
@@ -3510,10 +3441,10 @@
         <v>4</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J66" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K66" s="2">
         <v>43032</v>
@@ -3524,19 +3455,19 @@
         <v>52</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" t="s">
         <v>67</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F67" t="s">
-        <v>66</v>
       </c>
       <c r="G67" s="5">
         <v>24</v>
@@ -3545,10 +3476,10 @@
         <v>4</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J67" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K67" s="2">
         <v>43032</v>
@@ -3559,19 +3490,19 @@
         <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" t="s">
         <v>67</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F68" t="s">
-        <v>66</v>
       </c>
       <c r="G68" s="5">
         <v>42</v>
@@ -3580,10 +3511,10 @@
         <v>4</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J68" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K68" s="2">
         <v>43032</v>
@@ -3594,19 +3525,19 @@
         <v>54</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" t="s">
         <v>67</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F69" t="s">
-        <v>66</v>
       </c>
       <c r="G69" s="5">
         <v>48</v>
@@ -3615,10 +3546,10 @@
         <v>4</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J69" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K69" s="2">
         <v>43032</v>
@@ -3629,19 +3560,19 @@
         <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
         <v>67</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F70" t="s">
-        <v>66</v>
       </c>
       <c r="G70" s="5">
         <v>63</v>
@@ -3650,10 +3581,10 @@
         <v>4</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J70" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K70" s="2">
         <v>43032</v>
@@ -3664,19 +3595,19 @@
         <v>56</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" t="s">
         <v>67</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F71" t="s">
-        <v>66</v>
       </c>
       <c r="G71" s="5">
         <v>69</v>
@@ -3685,10 +3616,10 @@
         <v>4</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J71" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K71" s="2">
         <v>43032</v>
@@ -3696,22 +3627,22 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" t="s">
         <v>67</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F72" t="s">
-        <v>66</v>
       </c>
       <c r="G72" s="5">
         <v>69</v>
@@ -3720,10 +3651,10 @@
         <v>4</v>
       </c>
       <c r="I72" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J72" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K72" s="2">
         <v>43032</v>
@@ -3734,19 +3665,19 @@
         <v>57</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F73" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G73" s="5">
         <v>0</v>
@@ -3758,7 +3689,7 @@
         <v>40</v>
       </c>
       <c r="J73" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K73" s="2">
         <v>43032</v>
@@ -3769,19 +3700,19 @@
         <v>58</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F74" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G74" s="5">
         <v>18</v>
@@ -3793,7 +3724,7 @@
         <v>40</v>
       </c>
       <c r="J74" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K74" s="2">
         <v>43032</v>
@@ -3804,19 +3735,19 @@
         <v>59</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F75" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G75" s="5">
         <v>24</v>
@@ -3828,7 +3759,7 @@
         <v>40</v>
       </c>
       <c r="J75" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K75" s="2">
         <v>43032</v>
@@ -3839,19 +3770,19 @@
         <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F76" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G76" s="5">
         <v>42</v>
@@ -3863,7 +3794,7 @@
         <v>40</v>
       </c>
       <c r="J76" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K76" s="2">
         <v>43032</v>
@@ -3874,19 +3805,19 @@
         <v>61</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F77" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G77" s="5">
         <v>48</v>
@@ -3898,7 +3829,7 @@
         <v>40</v>
       </c>
       <c r="J77" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K77" s="2">
         <v>43032</v>
@@ -3909,19 +3840,19 @@
         <v>62</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F78" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G78" s="5">
         <v>63</v>
@@ -3933,7 +3864,7 @@
         <v>40</v>
       </c>
       <c r="J78" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K78" s="2">
         <v>43032</v>
@@ -3944,19 +3875,19 @@
         <v>63</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F79" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G79" s="5">
         <v>69</v>
@@ -3968,7 +3899,7 @@
         <v>40</v>
       </c>
       <c r="J79" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K79" s="2">
         <v>43032</v>
@@ -3976,22 +3907,22 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F80" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G80" s="5">
         <v>69</v>
@@ -4003,7 +3934,7 @@
         <v>40</v>
       </c>
       <c r="J80" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K80" s="2">
         <v>43032</v>
@@ -4011,22 +3942,22 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F81" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G81" s="5">
         <v>0</v>
@@ -4038,7 +3969,7 @@
         <v>40</v>
       </c>
       <c r="J81" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K81" s="2">
         <v>43038</v>
@@ -4046,22 +3977,22 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F82" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G82" s="5">
         <v>16</v>
@@ -4073,7 +4004,7 @@
         <v>40</v>
       </c>
       <c r="J82" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K82" s="2">
         <v>43038</v>
@@ -4081,22 +4012,22 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F83" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G83" s="5">
         <v>21</v>
@@ -4108,7 +4039,7 @@
         <v>40</v>
       </c>
       <c r="J83" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K83" s="2">
         <v>43038</v>
@@ -4116,22 +4047,22 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F84" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G84" s="5">
         <v>26</v>
@@ -4143,7 +4074,7 @@
         <v>40</v>
       </c>
       <c r="J84" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K84" s="2">
         <v>43038</v>
@@ -4151,22 +4082,22 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F85" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G85" s="5">
         <v>42</v>
@@ -4178,7 +4109,7 @@
         <v>40</v>
       </c>
       <c r="J85" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K85" s="2">
         <v>43038</v>
@@ -4186,22 +4117,22 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F86" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G86" s="5">
         <v>47</v>
@@ -4213,7 +4144,7 @@
         <v>40</v>
       </c>
       <c r="J86" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K86" s="2">
         <v>43038</v>
@@ -4221,22 +4152,22 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F87" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G87" s="5">
         <v>66</v>
@@ -4248,7 +4179,7 @@
         <v>40</v>
       </c>
       <c r="J87" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K87" s="2">
         <v>43038</v>
@@ -4256,22 +4187,22 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F88" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G88" s="5">
         <v>66</v>
@@ -4283,7 +4214,7 @@
         <v>40</v>
       </c>
       <c r="J88" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K88" s="2">
         <v>43038</v>
@@ -4291,22 +4222,22 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F89" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G89" s="5">
         <v>0</v>
@@ -4315,10 +4246,10 @@
         <v>4</v>
       </c>
       <c r="I89" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J89" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K89" s="2">
         <v>43038</v>
@@ -4326,22 +4257,22 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F90" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G90" s="5">
         <v>16</v>
@@ -4350,10 +4281,10 @@
         <v>4</v>
       </c>
       <c r="I90" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J90" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K90" s="2">
         <v>43038</v>
@@ -4361,22 +4292,22 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F91" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G91" s="5">
         <v>21</v>
@@ -4385,10 +4316,10 @@
         <v>4</v>
       </c>
       <c r="I91" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J91" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K91" s="2">
         <v>43038</v>
@@ -4396,22 +4327,22 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F92" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G92" s="5">
         <v>26</v>
@@ -4420,10 +4351,10 @@
         <v>4</v>
       </c>
       <c r="I92" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J92" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K92" s="2">
         <v>43038</v>
@@ -4431,22 +4362,22 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F93" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G93" s="5">
         <v>42</v>
@@ -4455,10 +4386,10 @@
         <v>4</v>
       </c>
       <c r="I93" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J93" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K93" s="2">
         <v>43038</v>
@@ -4466,22 +4397,22 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F94" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G94" s="5">
         <v>47</v>
@@ -4490,10 +4421,10 @@
         <v>4</v>
       </c>
       <c r="I94" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J94" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K94" s="2">
         <v>43038</v>
@@ -4501,22 +4432,22 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F95" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G95" s="5">
         <v>66</v>
@@ -4525,10 +4456,10 @@
         <v>4</v>
       </c>
       <c r="I95" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J95" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K95" s="2">
         <v>43038</v>
@@ -4536,22 +4467,22 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F96" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G96" s="5">
         <v>66</v>
@@ -4560,10 +4491,10 @@
         <v>4</v>
       </c>
       <c r="I96" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J96" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K96" s="2">
         <v>43038</v>
@@ -4571,10 +4502,10 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>21</v>
@@ -4583,10 +4514,10 @@
         <v>22</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F97" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G97" s="5">
         <v>0</v>
@@ -4595,10 +4526,10 @@
         <v>4</v>
       </c>
       <c r="I97" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J97" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K97" s="2">
         <v>43038</v>
@@ -4606,10 +4537,10 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>21</v>
@@ -4618,10 +4549,10 @@
         <v>22</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F98" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G98" s="5">
         <v>16</v>
@@ -4630,10 +4561,10 @@
         <v>4</v>
       </c>
       <c r="I98" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J98" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K98" s="2">
         <v>43038</v>
@@ -4641,10 +4572,10 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>21</v>
@@ -4653,10 +4584,10 @@
         <v>22</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F99" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G99" s="5">
         <v>21</v>
@@ -4665,10 +4596,10 @@
         <v>4</v>
       </c>
       <c r="I99" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J99" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K99" s="2">
         <v>43038</v>
@@ -4676,10 +4607,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>21</v>
@@ -4688,10 +4619,10 @@
         <v>22</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F100" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G100" s="5">
         <v>26</v>
@@ -4700,10 +4631,10 @@
         <v>4</v>
       </c>
       <c r="I100" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J100" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K100" s="2">
         <v>43038</v>
@@ -4711,10 +4642,10 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>21</v>
@@ -4723,10 +4654,10 @@
         <v>22</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F101" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G101" s="5">
         <v>42</v>
@@ -4735,10 +4666,10 @@
         <v>4</v>
       </c>
       <c r="I101" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J101" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K101" s="2">
         <v>43038</v>
@@ -4746,10 +4677,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>21</v>
@@ -4758,10 +4689,10 @@
         <v>22</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F102" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G102" s="5">
         <v>47</v>
@@ -4770,10 +4701,10 @@
         <v>4</v>
       </c>
       <c r="I102" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J102" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K102" s="2">
         <v>43038</v>
@@ -4781,10 +4712,10 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>21</v>
@@ -4793,10 +4724,10 @@
         <v>22</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F103" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G103" s="5">
         <v>66</v>
@@ -4805,10 +4736,10 @@
         <v>4</v>
       </c>
       <c r="I103" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J103" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K103" s="2">
         <v>43038</v>
@@ -4816,10 +4747,10 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>21</v>
@@ -4828,10 +4759,10 @@
         <v>22</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F104" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G104" s="5">
         <v>66</v>
@@ -4840,10 +4771,10 @@
         <v>4</v>
       </c>
       <c r="I104" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J104" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K104" s="2">
         <v>43038</v>
@@ -4851,22 +4782,22 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F105" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G105" s="5">
         <v>0</v>
@@ -4875,10 +4806,10 @@
         <v>4</v>
       </c>
       <c r="I105" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J105" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K105" s="2">
         <v>43060</v>
@@ -4886,22 +4817,22 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F106" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G106" s="5">
         <v>8</v>
@@ -4910,10 +4841,10 @@
         <v>4</v>
       </c>
       <c r="I106" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J106" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K106" s="2">
         <v>43060</v>
@@ -4921,22 +4852,22 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F107" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G107" s="5">
         <v>21</v>
@@ -4945,10 +4876,10 @@
         <v>4</v>
       </c>
       <c r="I107" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J107" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K107" s="2">
         <v>43060</v>
@@ -4956,22 +4887,22 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F108" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G108" s="5">
         <v>30</v>
@@ -4980,10 +4911,10 @@
         <v>4</v>
       </c>
       <c r="I108" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J108" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K108" s="2">
         <v>43060</v>
@@ -4991,22 +4922,22 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F109" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G109" s="5">
         <v>45</v>
@@ -5015,10 +4946,10 @@
         <v>4</v>
       </c>
       <c r="I109" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J109" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K109" s="2">
         <v>43060</v>
@@ -5026,22 +4957,22 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F110" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G110" s="5">
         <v>54</v>
@@ -5050,10 +4981,10 @@
         <v>4</v>
       </c>
       <c r="I110" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J110" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K110" s="2">
         <v>43060</v>
@@ -5061,22 +4992,22 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F111" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G111" s="5">
         <v>66</v>
@@ -5085,643 +5016,13 @@
         <v>4</v>
       </c>
       <c r="I111" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J111" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K111" s="2">
         <v>43060</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F112" t="s">
-        <v>164</v>
-      </c>
-      <c r="G112" s="5">
-        <v>0</v>
-      </c>
-      <c r="H112" t="s">
-        <v>4</v>
-      </c>
-      <c r="I112" t="s">
-        <v>72</v>
-      </c>
-      <c r="J112" t="s">
-        <v>101</v>
-      </c>
-      <c r="K112" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F113" t="s">
-        <v>164</v>
-      </c>
-      <c r="G113" s="5">
-        <v>6</v>
-      </c>
-      <c r="H113" t="s">
-        <v>4</v>
-      </c>
-      <c r="I113" t="s">
-        <v>72</v>
-      </c>
-      <c r="J113" t="s">
-        <v>101</v>
-      </c>
-      <c r="K113" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F114" t="s">
-        <v>164</v>
-      </c>
-      <c r="G114" s="5">
-        <v>21</v>
-      </c>
-      <c r="H114" t="s">
-        <v>4</v>
-      </c>
-      <c r="I114" t="s">
-        <v>72</v>
-      </c>
-      <c r="J114" t="s">
-        <v>101</v>
-      </c>
-      <c r="K114" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F115" t="s">
-        <v>164</v>
-      </c>
-      <c r="G115" s="5">
-        <v>30</v>
-      </c>
-      <c r="H115" t="s">
-        <v>4</v>
-      </c>
-      <c r="I115" t="s">
-        <v>72</v>
-      </c>
-      <c r="J115" t="s">
-        <v>101</v>
-      </c>
-      <c r="K115" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F116" t="s">
-        <v>164</v>
-      </c>
-      <c r="G116" s="5">
-        <v>45</v>
-      </c>
-      <c r="H116" t="s">
-        <v>4</v>
-      </c>
-      <c r="I116" t="s">
-        <v>72</v>
-      </c>
-      <c r="J116" t="s">
-        <v>101</v>
-      </c>
-      <c r="K116" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F117" t="s">
-        <v>164</v>
-      </c>
-      <c r="G117" s="5">
-        <v>54</v>
-      </c>
-      <c r="H117" t="s">
-        <v>4</v>
-      </c>
-      <c r="I117" t="s">
-        <v>72</v>
-      </c>
-      <c r="J117" t="s">
-        <v>101</v>
-      </c>
-      <c r="K117" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F118" t="s">
-        <v>164</v>
-      </c>
-      <c r="G118" s="5">
-        <v>70</v>
-      </c>
-      <c r="H118" t="s">
-        <v>4</v>
-      </c>
-      <c r="I118" t="s">
-        <v>72</v>
-      </c>
-      <c r="J118" t="s">
-        <v>101</v>
-      </c>
-      <c r="K118" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F119" t="s">
-        <v>164</v>
-      </c>
-      <c r="G119" s="5">
-        <v>70</v>
-      </c>
-      <c r="H119" t="s">
-        <v>4</v>
-      </c>
-      <c r="I119" t="s">
-        <v>72</v>
-      </c>
-      <c r="J119" t="s">
-        <v>113</v>
-      </c>
-      <c r="K119" s="2">
-        <v>43073</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F120" t="s">
-        <v>179</v>
-      </c>
-      <c r="G120" s="5">
-        <v>0</v>
-      </c>
-      <c r="H120" t="s">
-        <v>4</v>
-      </c>
-      <c r="I120" t="s">
-        <v>72</v>
-      </c>
-      <c r="J120" t="s">
-        <v>101</v>
-      </c>
-      <c r="K120" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F121" t="s">
-        <v>179</v>
-      </c>
-      <c r="G121" s="5">
-        <v>8</v>
-      </c>
-      <c r="H121" t="s">
-        <v>4</v>
-      </c>
-      <c r="I121" t="s">
-        <v>72</v>
-      </c>
-      <c r="J121" t="s">
-        <v>101</v>
-      </c>
-      <c r="K121" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F122" t="s">
-        <v>179</v>
-      </c>
-      <c r="G122" s="5">
-        <v>19</v>
-      </c>
-      <c r="H122" t="s">
-        <v>4</v>
-      </c>
-      <c r="I122" t="s">
-        <v>72</v>
-      </c>
-      <c r="J122" t="s">
-        <v>101</v>
-      </c>
-      <c r="K122" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F123" t="s">
-        <v>179</v>
-      </c>
-      <c r="G123" s="5">
-        <v>28</v>
-      </c>
-      <c r="H123" t="s">
-        <v>4</v>
-      </c>
-      <c r="I123" t="s">
-        <v>72</v>
-      </c>
-      <c r="J123" t="s">
-        <v>101</v>
-      </c>
-      <c r="K123" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F124" t="s">
-        <v>179</v>
-      </c>
-      <c r="G124" s="5">
-        <v>45</v>
-      </c>
-      <c r="H124" t="s">
-        <v>4</v>
-      </c>
-      <c r="I124" t="s">
-        <v>72</v>
-      </c>
-      <c r="J124" t="s">
-        <v>101</v>
-      </c>
-      <c r="K124" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F125" t="s">
-        <v>180</v>
-      </c>
-      <c r="G125" s="5">
-        <v>0</v>
-      </c>
-      <c r="H125" t="s">
-        <v>4</v>
-      </c>
-      <c r="I125" t="s">
-        <v>40</v>
-      </c>
-      <c r="J125" t="s">
-        <v>101</v>
-      </c>
-      <c r="K125" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F126" t="s">
-        <v>180</v>
-      </c>
-      <c r="G126" s="5">
-        <v>8</v>
-      </c>
-      <c r="H126" t="s">
-        <v>4</v>
-      </c>
-      <c r="I126" t="s">
-        <v>40</v>
-      </c>
-      <c r="J126" t="s">
-        <v>101</v>
-      </c>
-      <c r="K126" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F127" t="s">
-        <v>180</v>
-      </c>
-      <c r="G127" s="5">
-        <v>19</v>
-      </c>
-      <c r="H127" t="s">
-        <v>4</v>
-      </c>
-      <c r="I127" t="s">
-        <v>40</v>
-      </c>
-      <c r="J127" t="s">
-        <v>101</v>
-      </c>
-      <c r="K127" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F128" t="s">
-        <v>180</v>
-      </c>
-      <c r="G128" s="5">
-        <v>28</v>
-      </c>
-      <c r="H128" t="s">
-        <v>4</v>
-      </c>
-      <c r="I128" t="s">
-        <v>40</v>
-      </c>
-      <c r="J128" t="s">
-        <v>101</v>
-      </c>
-      <c r="K128" s="2">
-        <v>43108</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F129" t="s">
-        <v>180</v>
-      </c>
-      <c r="G129" s="5">
-        <v>45</v>
-      </c>
-      <c r="H129" t="s">
-        <v>4</v>
-      </c>
-      <c r="I129" t="s">
-        <v>40</v>
-      </c>
-      <c r="J129" t="s">
-        <v>101</v>
-      </c>
-      <c r="K129" s="2">
-        <v>43108</v>
       </c>
     </row>
   </sheetData>
@@ -5738,15 +5039,15 @@
     <hyperlink ref="A73" r:id="rId10"/>
     <hyperlink ref="A78" r:id="rId11"/>
     <hyperlink ref="A79" r:id="rId12"/>
-    <hyperlink ref="B57" r:id="rId13" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B57" r:id="rId13"/>
     <hyperlink ref="A89" r:id="rId14"/>
-    <hyperlink ref="B81" r:id="rId15" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B81" r:id="rId15"/>
     <hyperlink ref="A81" r:id="rId16"/>
     <hyperlink ref="A97" r:id="rId17"/>
     <hyperlink ref="A28" r:id="rId18"/>
     <hyperlink ref="B2" r:id="rId19"/>
     <hyperlink ref="B34" r:id="rId20"/>
-    <hyperlink ref="B104" r:id="rId21" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B104" r:id="rId21"/>
     <hyperlink ref="A2" r:id="rId22"/>
     <hyperlink ref="A3" r:id="rId23"/>
     <hyperlink ref="A12" r:id="rId24" display="\\carbon.research.sickkids.ca\OPRETTA\Operetta Processed OutPutFiles\Dataset_20170627_HD_CycD_6hrRESULTS"/>
@@ -5782,12 +5083,12 @@
     <hyperlink ref="A10" r:id="rId54"/>
     <hyperlink ref="A19" r:id="rId55"/>
     <hyperlink ref="A20" r:id="rId56"/>
-    <hyperlink ref="B67" r:id="rId57" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
-    <hyperlink ref="B65" r:id="rId58" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171024_D1_E1_P27.xlsx"/>
-    <hyperlink ref="B95" r:id="rId59" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171030_D1_E1_P27.xlsx"/>
+    <hyperlink ref="B67" r:id="rId57"/>
+    <hyperlink ref="B65" r:id="rId58"/>
+    <hyperlink ref="B95" r:id="rId59"/>
     <hyperlink ref="B29" r:id="rId60"/>
     <hyperlink ref="A106" r:id="rId61"/>
-    <hyperlink ref="B105" r:id="rId62" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx"/>
+    <hyperlink ref="B105" r:id="rId62"/>
     <hyperlink ref="B106:B111" r:id="rId63" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171120_cycE1_P27.xlsx"/>
     <hyperlink ref="A104" r:id="rId64"/>
     <hyperlink ref="A105" r:id="rId65"/>
@@ -5796,27 +5097,11 @@
     <hyperlink ref="A109" r:id="rId68"/>
     <hyperlink ref="A110" r:id="rId69"/>
     <hyperlink ref="A111" r:id="rId70"/>
-    <hyperlink ref="B112" r:id="rId71" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
-    <hyperlink ref="A112" r:id="rId72"/>
-    <hyperlink ref="B117" r:id="rId73" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
-    <hyperlink ref="B118" r:id="rId74" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
-    <hyperlink ref="B119" r:id="rId75" display="\\carbon.research.sickkids.ca\rkafri\Justin S\Experiments\Growth Rate\Plate map 20171204_cycE1.xlsx"/>
-    <hyperlink ref="A119" r:id="rId76"/>
-    <hyperlink ref="A122" r:id="rId77"/>
-    <hyperlink ref="A125" r:id="rId78"/>
-    <hyperlink ref="B120" r:id="rId79"/>
-    <hyperlink ref="B121:B127" r:id="rId80" display="\\carbon.research.sickkids.ca\rkafri\Justin_S\Experiments\Growth Rate\Plate map 20180108_cycE1_P27.xlsx"/>
-    <hyperlink ref="A120" r:id="rId81"/>
-    <hyperlink ref="A126" r:id="rId82"/>
-    <hyperlink ref="B123" r:id="rId83"/>
-    <hyperlink ref="B128" r:id="rId84"/>
-    <hyperlink ref="B124" r:id="rId85"/>
-    <hyperlink ref="B129" r:id="rId86"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId87"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
   <tableParts count="1">
-    <tablePart r:id="rId88"/>
+    <tablePart r:id="rId72"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>